<commit_message>
Avances Secuencia y pruebas
</commit_message>
<xml_diff>
--- a/sudoku/resultados.xlsx
+++ b/sudoku/resultados.xlsx
@@ -500,13 +500,13 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0.0013386</v>
+        <v>0.0143196</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0060631</v>
+        <v>0.008996000000000001</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0074017</v>
+        <v>0.0233156</v>
       </c>
       <c r="H2" t="n">
         <v>1</v>
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0.0011562</v>
+        <v>0.0033008</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0280476</v>
+        <v>0.029005</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0292038</v>
+        <v>0.0323058</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
@@ -586,13 +586,13 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0.0011539</v>
+        <v>0.0034801</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0135425</v>
+        <v>0.0189907</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0146964</v>
+        <v>0.0224708</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
@@ -629,13 +629,13 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0.0013686</v>
+        <v>0.0016799</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0127835</v>
+        <v>0.015511</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0141521</v>
+        <v>0.0171909</v>
       </c>
       <c r="H5" t="n">
         <v>1</v>
@@ -672,13 +672,13 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0.0011348</v>
+        <v>0.0017125</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0121439</v>
+        <v>0.0179787</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0132787</v>
+        <v>0.0196912</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -715,13 +715,13 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0.0014383</v>
+        <v>0.0021541</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0062517</v>
+        <v>0.0080588</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00769</v>
+        <v>0.0102129</v>
       </c>
       <c r="H7" t="n">
         <v>1</v>
@@ -761,10 +761,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="F8" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="G8" t="n">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
@@ -801,13 +801,13 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="F9" t="n">
         <v>0.001</v>
       </c>
       <c r="G9" t="n">
-        <v>0.009000000000000001</v>
+        <v>0.015</v>
       </c>
       <c r="H9" t="n">
         <v>1</v>
@@ -844,13 +844,13 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0.01</v>
+        <v>0.012</v>
       </c>
       <c r="F10" t="n">
         <v>0.001</v>
       </c>
       <c r="G10" t="n">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
@@ -887,13 +887,13 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.012</v>
       </c>
       <c r="F11" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="G11" t="n">
-        <v>0.011</v>
+        <v>0.013</v>
       </c>
       <c r="H11" t="n">
         <v>1</v>
@@ -930,13 +930,13 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.014</v>
       </c>
       <c r="F12" t="n">
         <v>0.001</v>
       </c>
       <c r="G12" t="n">
-        <v>0.009999999999999998</v>
+        <v>0.015</v>
       </c>
       <c r="H12" t="n">
         <v>1</v>
@@ -973,13 +973,13 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G13" t="n">
-        <v>0.008</v>
+        <v>0.015</v>
       </c>
       <c r="H13" t="n">
         <v>1</v>
@@ -1016,13 +1016,13 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0.0013456</v>
+        <v>0.0025464</v>
       </c>
       <c r="F14" t="n">
-        <v>0.007534</v>
+        <v>0.0152986</v>
       </c>
       <c r="G14" t="n">
-        <v>0.0088796</v>
+        <v>0.017845</v>
       </c>
       <c r="H14" t="n">
         <v>1</v>
@@ -1059,13 +1059,13 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0.0011532</v>
+        <v>0.0043354</v>
       </c>
       <c r="F15" t="n">
-        <v>0.0603492</v>
+        <v>0.12559</v>
       </c>
       <c r="G15" t="n">
-        <v>0.0615024</v>
+        <v>0.1299254</v>
       </c>
       <c r="H15" t="n">
         <v>1</v>
@@ -1102,13 +1102,13 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0.0011206</v>
+        <v>0.0030313</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0137368</v>
+        <v>0.0310622</v>
       </c>
       <c r="G16" t="n">
-        <v>0.0148574</v>
+        <v>0.0340935</v>
       </c>
       <c r="H16" t="n">
         <v>1</v>
@@ -1145,13 +1145,13 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0.0017951</v>
+        <v>0.0034796</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0152056</v>
+        <v>0.0394506</v>
       </c>
       <c r="G17" t="n">
-        <v>0.0170007</v>
+        <v>0.0429302</v>
       </c>
       <c r="H17" t="n">
         <v>1</v>
@@ -1188,13 +1188,13 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0.0011627</v>
+        <v>0.0281511</v>
       </c>
       <c r="F18" t="n">
-        <v>0.0133363</v>
+        <v>0.0378699</v>
       </c>
       <c r="G18" t="n">
-        <v>0.014499</v>
+        <v>0.066021</v>
       </c>
       <c r="H18" t="n">
         <v>1</v>
@@ -1231,13 +1231,13 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>0.00112</v>
+        <v>0.0031338</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0077695</v>
+        <v>0.0170736</v>
       </c>
       <c r="G19" t="n">
-        <v>0.0088895</v>
+        <v>0.0202074</v>
       </c>
       <c r="H19" t="n">
         <v>1</v>
@@ -1274,13 +1274,13 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0.007</v>
+        <v>0.019</v>
       </c>
       <c r="F20" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
       <c r="G20" t="n">
-        <v>0.009000000000000001</v>
+        <v>0.024</v>
       </c>
       <c r="H20" t="n">
         <v>1</v>
@@ -1317,13 +1317,13 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0.007</v>
+        <v>0.016</v>
       </c>
       <c r="F21" t="n">
-        <v>0.006</v>
+        <v>0.013</v>
       </c>
       <c r="G21" t="n">
-        <v>0.013</v>
+        <v>0.029</v>
       </c>
       <c r="H21" t="n">
         <v>1</v>
@@ -1360,13 +1360,13 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0.006</v>
+        <v>0.022</v>
       </c>
       <c r="F22" t="n">
-        <v>0.005</v>
+        <v>0.008</v>
       </c>
       <c r="G22" t="n">
-        <v>0.011</v>
+        <v>0.03</v>
       </c>
       <c r="H22" t="n">
         <v>1</v>
@@ -1403,13 +1403,13 @@
         </is>
       </c>
       <c r="E23" t="n">
+        <v>0.015</v>
+      </c>
+      <c r="F23" t="n">
         <v>0.008999999999999999</v>
       </c>
-      <c r="F23" t="n">
-        <v>0.005</v>
-      </c>
       <c r="G23" t="n">
-        <v>0.014</v>
+        <v>0.024</v>
       </c>
       <c r="H23" t="n">
         <v>1</v>
@@ -1446,13 +1446,13 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.021</v>
       </c>
       <c r="F24" t="n">
-        <v>0.006</v>
+        <v>0.011</v>
       </c>
       <c r="G24" t="n">
-        <v>0.015</v>
+        <v>0.032</v>
       </c>
       <c r="H24" t="n">
         <v>1</v>
@@ -1489,13 +1489,13 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.019</v>
       </c>
       <c r="F25" t="n">
-        <v>0.008</v>
+        <v>0.015</v>
       </c>
       <c r="G25" t="n">
-        <v>0.017</v>
+        <v>0.034</v>
       </c>
       <c r="H25" t="n">
         <v>1</v>
@@ -1532,13 +1532,13 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0.0009915</v>
+        <v>0.0043865</v>
       </c>
       <c r="F26" t="n">
-        <v>0.004415</v>
+        <v>0.009944700000000001</v>
       </c>
       <c r="G26" t="n">
-        <v>0.0054065</v>
+        <v>0.0143312</v>
       </c>
       <c r="H26" t="n">
         <v>21</v>
@@ -1575,13 +1575,13 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0.001146</v>
+        <v>0.002736</v>
       </c>
       <c r="F27" t="n">
-        <v>0.022478</v>
+        <v>0.0517939</v>
       </c>
       <c r="G27" t="n">
-        <v>0.023624</v>
+        <v>0.0545299</v>
       </c>
       <c r="H27" t="n">
         <v>21</v>
@@ -1618,13 +1618,13 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0.0016797</v>
+        <v>0.0024474</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0072657</v>
+        <v>0.0115114</v>
       </c>
       <c r="G28" t="n">
-        <v>0.008945399999999999</v>
+        <v>0.0139588</v>
       </c>
       <c r="H28" t="n">
         <v>21</v>
@@ -1661,13 +1661,13 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0.0011459</v>
+        <v>0.0024575</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0055517</v>
+        <v>0.0136257</v>
       </c>
       <c r="G29" t="n">
-        <v>0.0066976</v>
+        <v>0.0160832</v>
       </c>
       <c r="H29" t="n">
         <v>21</v>
@@ -1704,13 +1704,13 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0.0011251</v>
+        <v>0.0032042</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0063638</v>
+        <v>0.0125908</v>
       </c>
       <c r="G30" t="n">
-        <v>0.0074889</v>
+        <v>0.015795</v>
       </c>
       <c r="H30" t="n">
         <v>21</v>
@@ -1747,13 +1747,13 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0.0011244</v>
+        <v>0.0040657</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0046817</v>
+        <v>0.0126894</v>
       </c>
       <c r="G31" t="n">
-        <v>0.0058061</v>
+        <v>0.0167551</v>
       </c>
       <c r="H31" t="n">
         <v>21</v>
@@ -1790,13 +1790,13 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.018</v>
       </c>
       <c r="F32" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="G32" t="n">
-        <v>0.014</v>
+        <v>0.025</v>
       </c>
       <c r="H32" t="n">
         <v>21</v>
@@ -1833,13 +1833,13 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0.007</v>
+        <v>0.017</v>
       </c>
       <c r="F33" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="G33" t="n">
-        <v>0.01</v>
+        <v>0.022</v>
       </c>
       <c r="H33" t="n">
         <v>21</v>
@@ -1876,13 +1876,13 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.022</v>
       </c>
       <c r="F34" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G34" t="n">
-        <v>0.012</v>
+        <v>0.026</v>
       </c>
       <c r="H34" t="n">
         <v>21</v>
@@ -1919,13 +1919,13 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0.01</v>
+        <v>0.016</v>
       </c>
       <c r="F35" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="G35" t="n">
-        <v>0.013</v>
+        <v>0.02</v>
       </c>
       <c r="H35" t="n">
         <v>21</v>
@@ -1962,13 +1962,13 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0.008</v>
+        <v>0.02</v>
       </c>
       <c r="F36" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="G36" t="n">
-        <v>0.011</v>
+        <v>0.025</v>
       </c>
       <c r="H36" t="n">
         <v>21</v>
@@ -2005,13 +2005,13 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="F37" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="G37" t="n">
-        <v>0.012</v>
+        <v>0.019</v>
       </c>
       <c r="H37" t="n">
         <v>21</v>
@@ -2048,13 +2048,13 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0.0011387</v>
+        <v>0.005246</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0001551</v>
+        <v>0.0003067</v>
       </c>
       <c r="G38" t="n">
-        <v>0.0012938</v>
+        <v>0.0055527</v>
       </c>
       <c r="H38" t="n">
         <v>1</v>
@@ -2091,13 +2091,13 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0.001212</v>
+        <v>0.004866</v>
       </c>
       <c r="F39" t="n">
-        <v>0.000155</v>
+        <v>0.000298</v>
       </c>
       <c r="G39" t="n">
-        <v>0.001367</v>
+        <v>0.005163999999999999</v>
       </c>
       <c r="H39" t="n">
         <v>1</v>
@@ -2134,13 +2134,13 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0.0011339</v>
+        <v>0.0025165</v>
       </c>
       <c r="F40" t="n">
-        <v>0.00016</v>
+        <v>0.000301</v>
       </c>
       <c r="G40" t="n">
-        <v>0.0012939</v>
+        <v>0.0028175</v>
       </c>
       <c r="H40" t="n">
         <v>1</v>
@@ -2177,13 +2177,13 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0.0013289</v>
+        <v>0.0025043</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0002221</v>
+        <v>0.0003021</v>
       </c>
       <c r="G41" t="n">
-        <v>0.001551</v>
+        <v>0.0028064</v>
       </c>
       <c r="H41" t="n">
         <v>1</v>
@@ -2220,13 +2220,13 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0.0011734</v>
+        <v>0.0026975</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0001578</v>
+        <v>0.0004311</v>
       </c>
       <c r="G42" t="n">
-        <v>0.0013312</v>
+        <v>0.0031286</v>
       </c>
       <c r="H42" t="n">
         <v>1</v>
@@ -2263,13 +2263,13 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0.0016096</v>
+        <v>0.0041262</v>
       </c>
       <c r="F43" t="n">
-        <v>0.0002152</v>
+        <v>0.0002848</v>
       </c>
       <c r="G43" t="n">
-        <v>0.0018248</v>
+        <v>0.004411</v>
       </c>
       <c r="H43" t="n">
         <v>1</v>
@@ -2306,13 +2306,13 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G44" t="n">
-        <v>0.01</v>
+        <v>0.016</v>
       </c>
       <c r="H44" t="n">
         <v>1</v>
@@ -2349,13 +2349,13 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0.008</v>
+        <v>0.019</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
       </c>
       <c r="G45" t="n">
-        <v>0.008</v>
+        <v>0.019</v>
       </c>
       <c r="H45" t="n">
         <v>1</v>
@@ -2392,13 +2392,13 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0.01</v>
+        <v>0.019</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
       </c>
       <c r="G46" t="n">
-        <v>0.01</v>
+        <v>0.019</v>
       </c>
       <c r="H46" t="n">
         <v>1</v>
@@ -2435,13 +2435,13 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0.008</v>
+        <v>0.022</v>
       </c>
       <c r="F47" t="n">
         <v>0.001</v>
       </c>
       <c r="G47" t="n">
-        <v>0.009000000000000001</v>
+        <v>0.023</v>
       </c>
       <c r="H47" t="n">
         <v>1</v>
@@ -2478,13 +2478,13 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.017</v>
       </c>
       <c r="F48" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G48" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.018</v>
       </c>
       <c r="H48" t="n">
         <v>1</v>
@@ -2521,13 +2521,13 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0.01</v>
+        <v>0.016</v>
       </c>
       <c r="F49" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="G49" t="n">
-        <v>0.01</v>
+        <v>0.017</v>
       </c>
       <c r="H49" t="n">
         <v>1</v>

</xml_diff>